<commit_message>
final presentation + MVC + some rename
</commit_message>
<xml_diff>
--- a/Function Points Calculation/TimeSpentUC.xlsx
+++ b/Function Points Calculation/TimeSpentUC.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\WaterMe\Function Points Calculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulg\Documents\GitHub\WaterMe\Function Points Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14373" windowHeight="4993"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>UC</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Calculated time</t>
+  </si>
+  <si>
+    <t>Real time spent</t>
   </si>
 </sst>
 </file>
@@ -246,9 +252,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +270,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,7 +515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7445A5FC-6FB4-4E58-AAB4-08C0CF240C4E}" type="CELLRANGE">
+                    <a:fld id="{2685737C-7B68-44CF-9D74-B22E2D688812}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -541,7 +547,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82C386F1-3902-4C90-9561-A664D45D43BF}" type="CELLRANGE">
+                    <a:fld id="{E3586012-6112-4613-A061-D0AB41349D5B}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -606,7 +612,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7F22405-6B4E-4DA6-8B35-4A9F408C2BD6}" type="CELLRANGE">
+                    <a:fld id="{E0B5A4C9-4DCF-4BFF-88F0-CDBDAD79B7BA}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -639,7 +645,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9891C29B-44AB-44DF-B2EA-95D5D4E8F499}" type="CELLRANGE">
+                    <a:fld id="{41F5EE33-CEAD-445D-9334-74AB3AA3BA27}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -704,7 +710,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5564AA88-B578-48A0-92D2-DED4522FE2E1}" type="CELLRANGE">
+                    <a:fld id="{2AC86213-8314-4735-B054-D78083EE2F6E}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -737,7 +743,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74210EDF-D2ED-4C08-BA86-82BBD49CBB12}" type="CELLRANGE">
+                    <a:fld id="{F87B3569-1C56-422A-8714-B2515E602E6E}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -770,7 +776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D217D099-E064-4141-B176-DBDE46417B56}" type="CELLRANGE">
+                    <a:fld id="{5781305A-5E6F-4EC7-83F7-11375CDD4ED2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2173,41 +2179,41 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F56" sqref="F55:F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.87890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41015625" customWidth="1"/>
+    <col min="4" max="4" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.29296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5859375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.41015625" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="9" max="9" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="1:9" ht="25.7" x14ac:dyDescent="0.85">
+      <c r="C1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="A4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2236,190 +2242,190 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>8</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>10.25</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>0.2</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>0</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <f t="shared" ref="G7:G12" si="0">B7+C7+D7</f>
         <v>18.45</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>3.9</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>2.25</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>0.2</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>1</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>0</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <f t="shared" si="0"/>
         <v>5.45</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>9.36</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>1</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>1.6</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>0.2</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>0</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>11.52</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>2.5</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>28.25</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>0.2</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>2</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="16">
+      <c r="F10" s="13"/>
+      <c r="G10" s="15">
         <f t="shared" si="0"/>
         <v>30.95</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>16.899999999999999</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>3</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>6.5</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>0.2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>0</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <f t="shared" si="0"/>
         <v>9.6999999999999993</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <v>15.84</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>1</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>0.2</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>0</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>0</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="15">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>2.16</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:9" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="A14" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A16" s="9" t="s">
         <v>0</v>
       </c>
@@ -2448,125 +2454,170 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>1</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>1</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="15">
         <f>(H17-7.6783)/0.3396</f>
         <v>38.87426383981154</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="15">
         <v>20.88</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="43" x14ac:dyDescent="0.5">
       <c r="A18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>1</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <v>0</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="15">
         <f t="shared" ref="G18:G20" si="1">(H18-7.6783)/0.3396</f>
         <v>8.0144287396937575</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="15">
         <v>10.4</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>2</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="13">
         <v>0</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="15">
         <f t="shared" si="1"/>
         <v>11.312426383981153</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="15">
         <v>11.52</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="17">
         <v>1</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <v>0</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="15">
         <f t="shared" si="1"/>
         <v>4.9520023557126009</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="15">
         <v>9.36</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A53" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="2">
+        <v>38.9</v>
+      </c>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="2">
+        <v>8</v>
+      </c>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A55" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="2">
+        <v>11.3</v>
+      </c>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A56" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="2">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>